<commit_message>
Update readme and benchmarks
</commit_message>
<xml_diff>
--- a/Fast1BRC_results.xlsx
+++ b/Fast1BRC_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\1brc\Fast1BRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CF8004-BB84-4B1C-9D9C-F6FAE6DBF620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF92DA3-35CE-4120-9BFC-975917D88C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="5110" windowWidth="21090" windowHeight="15470" xr2:uid="{FFEB1670-7915-4E0C-BE10-E91D7BD0AB70}"/>
   </bookViews>
@@ -192,10 +192,10 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -536,7 +536,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -574,12 +574,12 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
@@ -587,14 +587,14 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10" t="s">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
@@ -626,16 +626,16 @@
         <v>5</v>
       </c>
       <c r="D6" s="5">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="E6" s="5">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="F6" s="5">
-        <v>1417</v>
+        <v>1405</v>
       </c>
       <c r="G6" s="5">
-        <v>1383</v>
+        <v>1373</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -650,13 +650,13 @@
         <v>864</v>
       </c>
       <c r="E7" s="5">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="F7" s="5">
         <v>1453</v>
       </c>
       <c r="G7" s="5">
-        <v>1406</v>
+        <v>1400</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -708,12 +708,12 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
@@ -721,14 +721,14 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="10"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
@@ -760,16 +760,16 @@
         <v>5</v>
       </c>
       <c r="D14" s="7">
-        <v>2813</v>
+        <v>2390</v>
       </c>
       <c r="E14" s="7">
-        <v>2299</v>
+        <v>2315</v>
       </c>
       <c r="F14" s="7">
-        <v>5442</v>
+        <v>3640</v>
       </c>
       <c r="G14" s="7">
-        <v>3582</v>
+        <v>3583</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -781,16 +781,16 @@
         <v>6</v>
       </c>
       <c r="D15" s="5">
-        <v>2126</v>
+        <v>2153</v>
       </c>
       <c r="E15" s="5">
-        <v>2068</v>
+        <v>2162</v>
       </c>
       <c r="F15" s="5">
-        <v>3243</v>
+        <v>3283</v>
       </c>
       <c r="G15" s="5">
-        <v>3204</v>
+        <v>3195</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -802,16 +802,16 @@
         <v>7</v>
       </c>
       <c r="D16" s="6">
-        <v>2688</v>
+        <v>2676</v>
       </c>
       <c r="E16" s="6">
-        <v>2609</v>
+        <v>2689</v>
       </c>
       <c r="F16" s="6">
-        <v>4451</v>
+        <v>4490</v>
       </c>
       <c r="G16" s="6">
-        <v>4340</v>
+        <v>4353</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -842,12 +842,12 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
@@ -855,14 +855,14 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10" t="s">
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="10"/>
+      <c r="G20" s="9"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
@@ -893,17 +893,17 @@
       <c r="C22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="6">
-        <v>1328</v>
+      <c r="D22" s="5">
+        <v>1244</v>
       </c>
       <c r="E22" s="5">
-        <v>1203</v>
-      </c>
-      <c r="F22" s="6">
-        <v>2969</v>
+        <v>1154</v>
+      </c>
+      <c r="F22" s="5">
+        <v>2851</v>
       </c>
       <c r="G22" s="5">
-        <v>2730</v>
+        <v>2798</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -915,16 +915,16 @@
         <v>6</v>
       </c>
       <c r="D23" s="5">
-        <v>1231</v>
-      </c>
-      <c r="E23" s="6">
-        <v>1360</v>
+        <v>1234</v>
+      </c>
+      <c r="E23" s="7">
+        <v>1310</v>
       </c>
       <c r="F23" s="5">
-        <v>2846</v>
+        <v>2832</v>
       </c>
       <c r="G23" s="5">
-        <v>2763</v>
+        <v>2792</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -936,16 +936,16 @@
         <v>7</v>
       </c>
       <c r="D24" s="6">
-        <v>1424</v>
+        <v>1419</v>
       </c>
       <c r="E24" s="6">
-        <v>1469</v>
+        <v>1444</v>
       </c>
       <c r="F24" s="6">
-        <v>3693</v>
+        <v>3755</v>
       </c>
       <c r="G24" s="6">
-        <v>3746</v>
+        <v>3804</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -976,12 +976,12 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
@@ -989,14 +989,14 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10" t="s">
+      <c r="E28" s="9"/>
+      <c r="F28" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G28" s="10"/>
+      <c r="G28" s="9"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
@@ -1027,17 +1027,17 @@
       <c r="C30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="7">
-        <v>1288</v>
+      <c r="D30" s="5">
+        <v>1206</v>
       </c>
       <c r="E30" s="7">
-        <v>1458</v>
+        <v>1229</v>
       </c>
       <c r="F30" s="5">
-        <v>2625</v>
+        <v>2711</v>
       </c>
       <c r="G30" s="7">
-        <v>2797</v>
+        <v>2760</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -1048,16 +1048,16 @@
         <v>6</v>
       </c>
       <c r="D31" s="5">
-        <v>1150</v>
+        <v>1159</v>
       </c>
       <c r="E31" s="5">
-        <v>1118</v>
+        <v>1138</v>
       </c>
       <c r="F31" s="5">
-        <v>2632</v>
+        <v>2686</v>
       </c>
       <c r="G31" s="5">
-        <v>2553</v>
+        <v>2549</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -1068,13 +1068,13 @@
         <v>7</v>
       </c>
       <c r="D32" s="6">
-        <v>1935</v>
+        <v>2017</v>
       </c>
       <c r="E32" s="6">
-        <v>1963</v>
+        <v>2031</v>
       </c>
       <c r="F32" s="6">
-        <v>4216</v>
+        <v>4138</v>
       </c>
       <c r="G32" s="6">
         <v>4240</v>
@@ -1128,18 +1128,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="D11:G11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>